<commit_message>
Matrice d'implication à jour
</commit_message>
<xml_diff>
--- a/Matrice Implication PROGAV.xlsx
+++ b/Matrice Implication PROGAV.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8811928-F19F-4A1E-BEF3-44DD370959E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B065BEB9-9E22-4CAB-B1EE-FF3D04600045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22140" windowHeight="6828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -15,19 +15,27 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>n°</t>
   </si>
   <si>
-    <t>date:</t>
-  </si>
-  <si>
     <t>REMARQUES:</t>
   </si>
   <si>
@@ -37,13 +45,7 @@
     <t>Tâche/Fonctionnalité/Fonction</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>Nom du/des Codeurs</t>
-  </si>
-  <si>
-    <t>MEMBRES DE L'EQUIPE:</t>
   </si>
   <si>
     <t>Nom 
@@ -51,6 +53,63 @@
   </si>
   <si>
     <t>MATRICE D'IMPLICATION : PROJET PROGAV</t>
+  </si>
+  <si>
+    <t>ENSemenCe</t>
+  </si>
+  <si>
+    <t>date: 23/05/25</t>
+  </si>
+  <si>
+    <t>MEMBRES DE L'EQUIPE: Cauzid Hugo / Valvin Émilie</t>
+  </si>
+  <si>
+    <t>Classee Plante</t>
+  </si>
+  <si>
+    <t>Classee Terrain</t>
+  </si>
+  <si>
+    <t>Classes héritées de Plante</t>
+  </si>
+  <si>
+    <t>Classes Dune, Herbeux, Jungle, Rocheux</t>
+  </si>
+  <si>
+    <t>Classe Simulation</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>Rapport</t>
+  </si>
+  <si>
+    <t>Cauzid / Valvin</t>
+  </si>
+  <si>
+    <t>Valvin</t>
+  </si>
+  <si>
+    <t>Classe Ratiboiseur</t>
+  </si>
+  <si>
+    <t>Cauzid</t>
+  </si>
+  <si>
+    <t>10 / 90</t>
+  </si>
+  <si>
+    <t>50 / 50</t>
+  </si>
+  <si>
+    <t>85 / 15</t>
+  </si>
+  <si>
+    <t>60 / 40</t>
+  </si>
+  <si>
+    <t>80 / 20</t>
   </si>
 </sst>
 </file>
@@ -338,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -382,6 +441,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -415,19 +480,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -710,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:E28"/>
+  <dimension ref="B1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,59 +790,65 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+    </row>
+    <row r="4" spans="2:5" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-    </row>
-    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5" ht="39.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>3</v>
+      <c r="E6" s="16" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="28" t="s">
-        <v>5</v>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
@@ -788,44 +856,70 @@
         <f>1+B7</f>
         <v>2</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="29"/>
+      <c r="C8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
-        <f t="shared" ref="B9:B21" si="0">1+B8</f>
+        <f>1+B8</f>
         <v>3</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="29"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B10:B20" si="0">1+B9</f>
         <v>4</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="29"/>
+      <c r="C10" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="29"/>
+      <c r="C11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="E12" s="29"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
@@ -833,18 +927,30 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="29"/>
+      <c r="C13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="29"/>
+      <c r="C14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="4">
@@ -891,31 +997,26 @@
       <c r="D19" s="7"/>
       <c r="E19" s="29"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="29"/>
-    </row>
-    <row r="21" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="4">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="30"/>
+      <c r="E20" s="31"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="10"/>
@@ -933,15 +1034,11 @@
       <c r="B26" s="10"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="10"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="11"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="3"/>
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>